<commit_message>
Hot end thermistor modified
</commit_message>
<xml_diff>
--- a/COLLECTED DATA/Thermistor Data.xlsx
+++ b/COLLECTED DATA/Thermistor Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Morroway\Documents\.A\Projects\3D-PRINTER\COLLECTED DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{29A45D85-BA9C-4FE0-86D4-3D4D70C581F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6381B0-50CB-4301-BCF5-B5A1FB11C017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="375" windowWidth="25440" windowHeight="15270" activeTab="1" xr2:uid="{759ECCC0-DE5A-4357-9E7D-57BD42931C1A}"/>
   </bookViews>
@@ -81,6 +81,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.000E+00"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -111,9 +114,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2930,14 +2935,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80D1B1EC-0E93-40C4-BA77-021297BD0124}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -3149,14 +3156,18 @@
       </c>
       <c r="F22">
         <f>(E23-E22)/(D23-D22)</f>
-        <v>2.6775316788488652E-4</v>
+        <v>2.6841735657041861E-4</v>
       </c>
       <c r="G22">
         <f>E22-(G23+D22^2*G24)*D22</f>
-        <v>7.3155509593590684E-4</v>
+        <v>7.2636382072754002E-4</v>
       </c>
       <c r="H22">
-        <v>40000</v>
+        <f>(3.3/65536)*I22</f>
+        <v>2.5177001953125</v>
+      </c>
+      <c r="I22">
+        <v>50000</v>
       </c>
       <c r="L22">
         <v>3.3</v>
@@ -3173,12 +3184,12 @@
         <v>5</v>
       </c>
       <c r="D23">
-        <f>LN(B14*1000)</f>
-        <v>11.297874083553355</v>
+        <f>LN(B13*1000)</f>
+        <v>11.512925464970229</v>
       </c>
       <c r="E23">
-        <f>1/(A14+272.15)</f>
-        <v>3.3096144299189145E-3</v>
+        <f>1/(A13+272.15)</f>
+        <v>3.3653037186606094E-3</v>
       </c>
       <c r="F23">
         <f>(E24-E22)/(D24-D22)</f>
@@ -3186,7 +3197,11 @@
       </c>
       <c r="G23">
         <f>F22-G24*(D22^2+D22*D23+D23^2)</f>
-        <v>2.1448464543221649E-4</v>
+        <v>2.1523079640187122E-4</v>
+      </c>
+      <c r="H23">
+        <f>H22/((3.3-H22)/H24)</f>
+        <v>32183.316168898051</v>
       </c>
       <c r="L23">
         <f>2^12</f>
@@ -3211,9 +3226,12 @@
         <f>1/(A30+272.15)</f>
         <v>2.6167735182519953E-3</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="2">
         <f>((F23-F22)/(D24-D23))*(D22+D23+D24)^-1</f>
-        <v>1.0737165671392453E-7</v>
+        <v>1.0550644660502131E-7</v>
+      </c>
+      <c r="H24">
+        <v>10000</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
@@ -3239,9 +3257,9 @@
       <c r="B27">
         <v>7.5730000000000004</v>
       </c>
-      <c r="D27">
-        <f>1/(G22+G23*LN(H22)+G24*LN(H22)^3)-272.15</f>
-        <v>47.12153569583802</v>
+      <c r="D27" s="3">
+        <f>1/(G22+G23*LN(H23)+G24*LN(H23)^3)-272.15</f>
+        <v>52.709069265363382</v>
       </c>
       <c r="E27" t="s">
         <v>12</v>

</xml_diff>